<commit_message>
Updates and added files
</commit_message>
<xml_diff>
--- a/elesa 19-20/ID & tshirts/Assistant Pending List.xlsx
+++ b/elesa 19-20/ID & tshirts/Assistant Pending List.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JASUS\Music\ELESA\ID &amp; tshirts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JASUS\Music\ELESA\elesa 19-20\ID &amp; tshirts\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,10 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="39">
-  <si>
-    <t>Offline</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="40">
   <si>
     <t>M</t>
   </si>
@@ -144,6 +141,12 @@
   </si>
   <si>
     <t>Technical director</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Remaining</t>
   </si>
 </sst>
 </file>
@@ -496,7 +499,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="E4" sqref="E4:E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -511,274 +514,274 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>0</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>0</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>0</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>0</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>0</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>0</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>0</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>0</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>0</v>
+        <v>4</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E11" s="3" t="s">
         <v>0</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E12" s="3" t="s">
         <v>0</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>0</v>
+        <v>4</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E15" s="2" t="s">
         <v>0</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>38</v>
-      </c>
       <c r="D16" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E16" s="3" t="s">
         <v>0</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>